<commit_message>
Commited with colour and lang changes + new data to excel
</commit_message>
<xml_diff>
--- a/necropolis/cemetryCoords.xlsx
+++ b/necropolis/cemetryCoords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodovid\web\necropolis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A033BFF-9E3F-49CF-8E28-D05E918A0F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD13E3A-FF80-4B3D-AF5F-28F3E1B12098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="206">
   <si>
     <t>ПІБ</t>
   </si>
@@ -202,6 +202,447 @@
   </si>
   <si>
     <t>В нижній частині цвинтаря</t>
+  </si>
+  <si>
+    <t>Онода Анатолій Іванович</t>
+  </si>
+  <si>
+    <t>1932 - 1981</t>
+  </si>
+  <si>
+    <t>43.814444, 132.018056</t>
+  </si>
+  <si>
+    <t>http://skorbim.com/%D0%BC%D0%B5%D0%BC%D0%BE%D1%80%D0%B8%D0%B0%D0%BB/%D0%BE%D0%BD%D0%BE%D0%B4%D0%B0_%D0%B0%D0%BD%D0%B0%D1%82%D0%BE%D0%BB%D0%B8%D0%B9_%D0%B8%D0%B2%D0%B0%D0%BD%D0%BE%D0%B2%D0%B8%D1%87.html</t>
+  </si>
+  <si>
+    <t>Цвинтар міста Уссурійська, Зелений Клин</t>
+  </si>
+  <si>
+    <t>Онода Ольга Порфирівна</t>
+  </si>
+  <si>
+    <t>1908 - 1978</t>
+  </si>
+  <si>
+    <t>43.814454, 132.018076</t>
+  </si>
+  <si>
+    <t>43.814464, 132.018096</t>
+  </si>
+  <si>
+    <t>43.814474, 132.018116</t>
+  </si>
+  <si>
+    <t>http://skorbim.com/%D0%BC%D0%B5%D0%BC%D0%BE%D1%80%D0%B8%D0%B0%D0%BB/%D0%BE%D0%BD%D0%BE%D0%B4%D0%B0_%D0%BE%D0%BB%D1%8C%D0%B3%D0%B0_%D0%BF%D0%BE%D1%80%D1%84%D0%B8%D1%80%D1%8C%D0%B5%D0%B2%D0%BD%D0%B0.html</t>
+  </si>
+  <si>
+    <t>http://skorbim.com/%D0%BC%D0%B5%D0%BC%D0%BE%D1%80%D0%B8%D0%B0%D0%BB/%D0%B1%D1%83%D1%80%D1%8F%D0%BA%D0%BE%D0%B2%D0%B0_%D0%BD%D0%B8%D0%BD%D0%B0_%D0%B8%D0%B2%D0%B0%D0%BD%D0%BE%D0%B2%D0%BD%D0%B0.html</t>
+  </si>
+  <si>
+    <t>Бурякова (Онода) Ніна Іванівна</t>
+  </si>
+  <si>
+    <t>1936 - 2010</t>
+  </si>
+  <si>
+    <t>Буряков Геннадій Євгенович</t>
+  </si>
+  <si>
+    <t>1938 - 2003</t>
+  </si>
+  <si>
+    <t>http://skorbim.com/%D0%BC%D0%B5%D0%BC%D0%BE%D1%80%D0%B8%D0%B0%D0%BB/%D0%B1%D1%83%D1%80%D1%8F%D0%BA%D0%BE%D0%B2_%D0%B3%D0%B5%D0%BD%D0%BD%D0%B0%D0%B4%D0%B8%D0%B9_%D0%B5%D0%B2%D0%B3%D0%B5%D0%BD%D1%8C%D0%B5%D0%B2%D0%B8%D1%87.html</t>
+  </si>
+  <si>
+    <t>Тарасенко Єфросинія Григорівна</t>
+  </si>
+  <si>
+    <t>49.888015, 24.024378</t>
+  </si>
+  <si>
+    <t>Поле 16В. До неї підхоронений ненароджений Жилочкін Леонід Максимович</t>
+  </si>
+  <si>
+    <t>1907 - 1999</t>
+  </si>
+  <si>
+    <t>Лазар Микола Олексійович</t>
+  </si>
+  <si>
+    <t>1926 - 1999</t>
+  </si>
+  <si>
+    <t>49.888018, 24.024313</t>
+  </si>
+  <si>
+    <t>Треба уточнити, хто це</t>
+  </si>
+  <si>
+    <t>Сінельніков Леонід Степанович</t>
+  </si>
+  <si>
+    <t>Сінельнікова Уляна Макарівна</t>
+  </si>
+  <si>
+    <t>1952 - 2005</t>
+  </si>
+  <si>
+    <t>1915 - 2000</t>
+  </si>
+  <si>
+    <t>49.888132, 24.024295</t>
+  </si>
+  <si>
+    <t>49.888115, 24.024291</t>
+  </si>
+  <si>
+    <t>Разом з Сінельніковою Уляною Макарівною</t>
+  </si>
+  <si>
+    <t>Разом з Сінельніковим Леонідом Степановичем</t>
+  </si>
+  <si>
+    <t>49.888048, 24.024019</t>
+  </si>
+  <si>
+    <t>49.888060, 24.024018</t>
+  </si>
+  <si>
+    <t>Болотнікова Лідія Георгіївна</t>
+  </si>
+  <si>
+    <t>Болотніков Володимир Тимофійович</t>
+  </si>
+  <si>
+    <t>1917 - 1999</t>
+  </si>
+  <si>
+    <t>1927 - 2004</t>
+  </si>
+  <si>
+    <t>Разом з чоловіком Володимиром</t>
+  </si>
+  <si>
+    <t>Разом з жінкою Лідією</t>
+  </si>
+  <si>
+    <t>Болотніков Геннадій Володимирович</t>
+  </si>
+  <si>
+    <t>1947 - 2000</t>
+  </si>
+  <si>
+    <t>49.888063, 24.024075</t>
+  </si>
+  <si>
+    <t>За своїми батьками, під деревом</t>
+  </si>
+  <si>
+    <t>49.888174, 24.023846</t>
+  </si>
+  <si>
+    <t>49.888156, 24.023836</t>
+  </si>
+  <si>
+    <t>Савелко Пилип Петрович</t>
+  </si>
+  <si>
+    <t>1913 - 2001</t>
+  </si>
+  <si>
+    <t>1918 - 2008</t>
+  </si>
+  <si>
+    <t>Савелко Анна Федорівна</t>
+  </si>
+  <si>
+    <t>Болотніков Віктор Володимирович</t>
+  </si>
+  <si>
+    <t>1952 - 2004</t>
+  </si>
+  <si>
+    <t>49.888197, 24.024830</t>
+  </si>
+  <si>
+    <t>Похований окремо від родини, трошки на горі</t>
+  </si>
+  <si>
+    <t>Проворна (Косицька) Олександра Полікарпівна</t>
+  </si>
+  <si>
+    <t>1920 - 1998</t>
+  </si>
+  <si>
+    <t>Шура</t>
+  </si>
+  <si>
+    <t>49.887841, 24.026662</t>
+  </si>
+  <si>
+    <t>Проворний Макар Адамович</t>
+  </si>
+  <si>
+    <t>Костя</t>
+  </si>
+  <si>
+    <t>1914 - 1989</t>
+  </si>
+  <si>
+    <t>49.889531, 24.028420</t>
+  </si>
+  <si>
+    <t>Кернер (Кореневська) Наталія Миколаївна</t>
+  </si>
+  <si>
+    <t>1950 - 2022</t>
+  </si>
+  <si>
+    <t>Троє поховані в ряд</t>
+  </si>
+  <si>
+    <t>Кореневська Пелагія Гаврилівна</t>
+  </si>
+  <si>
+    <t>1929 - 2013</t>
+  </si>
+  <si>
+    <t>Кореневський Микола Андрійович</t>
+  </si>
+  <si>
+    <t>1919 - 1997</t>
+  </si>
+  <si>
+    <t>Трофименко Марія Василівна</t>
+  </si>
+  <si>
+    <t>Подарувала дачу</t>
+  </si>
+  <si>
+    <t>Чоловік Трофименко Марії Василівни, з Кубані</t>
+  </si>
+  <si>
+    <t>Трофименко Григорій Сергійович</t>
+  </si>
+  <si>
+    <t>1922 - 2003</t>
+  </si>
+  <si>
+    <t>1927 - 1994</t>
+  </si>
+  <si>
+    <t>49.894307, 24.024030</t>
+  </si>
+  <si>
+    <t>49.894311, 24.023971</t>
+  </si>
+  <si>
+    <t>49.889520, 24.029190</t>
+  </si>
+  <si>
+    <t>49.889540, 24.029191</t>
+  </si>
+  <si>
+    <t>49.889560, 24.029191</t>
+  </si>
+  <si>
+    <t>Царьков Іван Олександрович</t>
+  </si>
+  <si>
+    <t>1908 - 1962</t>
+  </si>
+  <si>
+    <t>1911 - 1995</t>
+  </si>
+  <si>
+    <t>1936 - 2012</t>
+  </si>
+  <si>
+    <t>Царькова Параскева Максимівна</t>
+  </si>
+  <si>
+    <t>Царькова Ніна Іванівна</t>
+  </si>
+  <si>
+    <t>49.850260, 23.997774</t>
+  </si>
+  <si>
+    <t>49.850263, 23.997761</t>
+  </si>
+  <si>
+    <t>Янівський, м. Львів</t>
+  </si>
+  <si>
+    <t>Батько Ніни Іванівни</t>
+  </si>
+  <si>
+    <t>Матір Ніни Іванівни</t>
+  </si>
+  <si>
+    <t>Матір Балабаєвої Світлани</t>
+  </si>
+  <si>
+    <t>49.850252, 23.997775</t>
+  </si>
+  <si>
+    <t>Петрова Анна Андріївна</t>
+  </si>
+  <si>
+    <t>1885 - 1966</t>
+  </si>
+  <si>
+    <t>Веселов Микола Полікарпович</t>
+  </si>
+  <si>
+    <t>1914 - 1995</t>
+  </si>
+  <si>
+    <t>1924 - 2019</t>
+  </si>
+  <si>
+    <t>Веселова (Петрова) Марія Василівна</t>
+  </si>
+  <si>
+    <t>49.853142, 23.996840</t>
+  </si>
+  <si>
+    <t>Перша від дороги, поле 45</t>
+  </si>
+  <si>
+    <t>Другий від дороги, поле 45</t>
+  </si>
+  <si>
+    <t>Третя від дороги, поле 45</t>
+  </si>
+  <si>
+    <t>49.853149, 23.996828</t>
+  </si>
+  <si>
+    <t>49.853158, 23.996808</t>
+  </si>
+  <si>
+    <t>Ловцус Надія Юріївна</t>
+  </si>
+  <si>
+    <t>Невідомо</t>
+  </si>
+  <si>
+    <t>Таблички нема - синій хрест навпроти гробівця Габів</t>
+  </si>
+  <si>
+    <t>49.852099, 23.994261</t>
+  </si>
+  <si>
+    <t>Суботін Леонід Степанович</t>
+  </si>
+  <si>
+    <t>1906 - 1963</t>
+  </si>
+  <si>
+    <t>49.852351, 23.993808</t>
+  </si>
+  <si>
+    <t>Потапенко Валентин Володимирович</t>
+  </si>
+  <si>
+    <t>1937 - 1989</t>
+  </si>
+  <si>
+    <t>1972 - 2019</t>
+  </si>
+  <si>
+    <t>Потапенко Костянтин Валентинович</t>
+  </si>
+  <si>
+    <t>Всі Суботіни</t>
+  </si>
+  <si>
+    <t>49.852348, 23.993813</t>
+  </si>
+  <si>
+    <t>49.852347, 23.993800</t>
+  </si>
+  <si>
+    <t>Суботіна Варвара Костянтинівна</t>
+  </si>
+  <si>
+    <t>1912 - 1956</t>
+  </si>
+  <si>
+    <t>Ближче до дороги</t>
+  </si>
+  <si>
+    <t>Суботін Георгій Леонідович</t>
+  </si>
+  <si>
+    <t>1947 - 1993</t>
+  </si>
+  <si>
+    <t>49.852363, 23.993782</t>
+  </si>
+  <si>
+    <t>49.852357, 23.993778</t>
+  </si>
+  <si>
+    <t>Воронич Василь Демидович</t>
+  </si>
+  <si>
+    <t>1921 - 1988</t>
+  </si>
+  <si>
+    <t>1926 - 2018</t>
+  </si>
+  <si>
+    <t>Воронич Олександра Герасимівна</t>
+  </si>
+  <si>
+    <t>Батько Воронича Василя Васильовича</t>
+  </si>
+  <si>
+    <t>Матір Воронича Василя Васильовича</t>
+  </si>
+  <si>
+    <t>49.852079, 23.993423</t>
+  </si>
+  <si>
+    <t>49.852084, 23.993403</t>
+  </si>
+  <si>
+    <t>50.036292, 28.406467</t>
+  </si>
+  <si>
+    <t>Старообрядницький, с. Пилипи, Житомирська обл.</t>
+  </si>
+  <si>
+    <t>1863 - 1980</t>
+  </si>
+  <si>
+    <t>Можлива похибка дати народження в кілька років</t>
+  </si>
+  <si>
+    <t>Косицька (Веселова) Мотрона Моїсеївна</t>
+  </si>
+  <si>
+    <t>50.036807, 28.406375</t>
+  </si>
+  <si>
+    <t>Косицький Полікарп Феофілактович</t>
+  </si>
+  <si>
+    <t>1956 - 1933</t>
+  </si>
+  <si>
+    <t>Без табличок. Прямий зелений хрест. Поруч з сином Анникієм</t>
+  </si>
+  <si>
+    <t>Косицький Анникій Полікарпович</t>
+  </si>
+  <si>
+    <t>50.036841, 28.406364</t>
+  </si>
+  <si>
+    <t>Випадково застрелився, допомагав партизанам в Другу Світову Війну</t>
   </si>
 </sst>
 </file>
@@ -238,18 +679,12 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,11 +699,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -549,293 +987,939 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="53.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="41.77734375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="43.5546875" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="D4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+    <row r="16" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="2" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added texts, other updates
</commit_message>
<xml_diff>
--- a/necropolis/cemetryCoords.xlsx
+++ b/necropolis/cemetryCoords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\rodovid\web\necropolis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FD13E3A-FF80-4B3D-AF5F-28F3E1B12098}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BA7C25-6D7E-4FF8-9A40-B37D8D791CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>Голосківський, м. Львів</t>
   </si>
   <si>
-    <t>Початок 43 поля</t>
-  </si>
-  <si>
     <t>Поважук Георгій Олександрович</t>
   </si>
   <si>
@@ -643,6 +640,9 @@
   </si>
   <si>
     <t>Випадково застрелився, допомагав партизанам в Другу Світову Війну</t>
+  </si>
+  <si>
+    <t>Початок 42 поля</t>
   </si>
 </sst>
 </file>
@@ -990,8 +990,8 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E55" sqref="E55"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1026,16 +1026,16 @@
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1043,16 +1043,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1060,16 +1060,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1077,849 +1077,849 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="110.4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C24" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="2" t="s">
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="C35" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="D37" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C39" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>148</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>154</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>156</v>
-      </c>
       <c r="C42" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>171</v>
-      </c>
       <c r="D45" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>173</v>
-      </c>
       <c r="C46" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="B50" s="2" t="s">
-        <v>187</v>
-      </c>
       <c r="C50" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>